<commit_message>
Fixed issue 2, 5, 7, 8, 12 and 13
TFS Changeset 2373: http://wtrxtfs2013.watertrax.local:8080/tfs/Linko/LinkoApplications/_versionControl/changeset/2373 

Workitems:
[8594] Coding- Implement Fix for Issue 2,5,7,8, 9,12 and 13
TFS: http://wtrxtfs2013.watertrax.local:8080/tfs/Linko/WorkItemTracking/WorkItem.aspx?artifactMoniker=8594 
Jira: https://aquaticinformatics.atlassian.net/issues/?jql=project%20%3D%20LINKO%20and%20tfsissueid~8594
</commit_message>
<xml_diff>
--- a/Linko.LinkoExchange.Web/Resources/SampleImportInstruction.xlsx
+++ b/Linko.LinkoExchange.Web/Resources/SampleImportInstruction.xlsx
@@ -8,26 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\LinkoApplications\Development\LinkoExchange\Linko.LinkoExchange.Web\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9542C153-0FD6-472B-B26C-3314C82C13EB}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{17F2FD19-6F23-4EE6-9708-CEFBBE6F1C61}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9135" tabRatio="764" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Descriptions" sheetId="14" r:id="rId1"/>
     <sheet name="Authority Settings" sheetId="15" r:id="rId2"/>
-    <sheet name="Data Example" sheetId="12" r:id="rId3"/>
-    <sheet name="Data Rules" sheetId="9" r:id="rId4"/>
-    <sheet name="How the Import Works" sheetId="11" r:id="rId5"/>
-    <sheet name="Data Example with Mass Loadings" sheetId="13" r:id="rId6"/>
+    <sheet name="Data Rules" sheetId="9" r:id="rId3"/>
+    <sheet name="Data Example" sheetId="12" r:id="rId4"/>
+    <sheet name="Data Example with Mass Loadings" sheetId="13" r:id="rId5"/>
+    <sheet name="How the Import Works" sheetId="11" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_Toc447789677" localSheetId="3">'Data Rules'!$A$4</definedName>
-    <definedName name="_Toc447789678" localSheetId="3">'Data Rules'!$A$10</definedName>
-    <definedName name="_Toc447789679" localSheetId="3">'Data Rules'!#REF!</definedName>
-    <definedName name="_Toc447789680" localSheetId="3">'Data Rules'!$A$13</definedName>
-    <definedName name="_Toc447789681" localSheetId="3">'Data Rules'!#REF!</definedName>
-    <definedName name="_Toc447789682" localSheetId="3">'Data Rules'!#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">'Data Rules'!$A$4:$A$20</definedName>
+    <definedName name="_Toc447789677" localSheetId="2">'Data Rules'!$A$4</definedName>
+    <definedName name="_Toc447789678" localSheetId="2">'Data Rules'!$A$10</definedName>
+    <definedName name="_Toc447789679" localSheetId="2">'Data Rules'!#REF!</definedName>
+    <definedName name="_Toc447789680" localSheetId="2">'Data Rules'!$A$13</definedName>
+    <definedName name="_Toc447789681" localSheetId="2">'Data Rules'!#REF!</definedName>
+    <definedName name="_Toc447789682" localSheetId="2">'Data Rules'!#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Data Rules'!$A$4:$A$20</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -247,9 +247,6 @@
 A file can contain results for multiple samples and LinkoExchange will automatically group those results into Samples using these fields.</t>
   </si>
   <si>
-    <t>Flow</t>
-  </si>
-  <si>
     <t>250000</t>
   </si>
   <si>
@@ -703,6 +700,399 @@
     <t>Required Fields</t>
   </si>
   <si>
+    <t>It is recommended that data for the optional fields also be included if it is available.  Data contained in columns indicated with ** will not be stored in LinkoExchange as those data elements are not currently supported, but when support is added for these columns, the data will import automatically.
+Columns indicated with ** can be excluded from the file completely if desired.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This is used to identify the differences between the various samples an Industry takes. What is required here is defined by the Authority.  See the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Authority Settings</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tab for a list of valid Sample Types and consult the Industry or Authority on when to use a particular type.
+Sample Type is a </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Recommended</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> field, see </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Recommended Fields</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> above for more details.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>LinkoExchange will accept the following combinations of values for the Result and Result Qualifier fields</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>depending on the Authorities settings:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+     </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Result</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =  0.098 (any numeric value) and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Result Qualifier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is blank
+     </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Result</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =  0.098 (any numeric value) and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Result Qualifier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is &lt; (result is less than 0.098 detection limit)
+     </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Result</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =  200 (any numeric value) and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Result Qualifier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is &gt; (result is greater than 200 detection limit)
+     </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Result</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = blank and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Result Qualifier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is ND (for non detect)
+     </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Result</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = blank and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Result Qualifier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is NF (for no flow, no sample taken)
+The combinations allowed is determined by the Authority.  See the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Authority Settings </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tab for a list of valid Result Qualifiers.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">&lt;orgname&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>accepts the following values for these fields.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">See the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Data Rules</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tab for more details.</t>
+    </r>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Fields identified as </t>
     </r>
@@ -742,16 +1132,12 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">  Some Required fields can be left blank if the row contains the Flow result that is being used to calculate Mass Loadings.  See Mass Loadings and Authority Required Fields below for more information.</t>
-    </r>
-  </si>
-  <si>
-    <t>It is recommended that data for the optional fields also be included if it is available.  Data contained in columns indicated with ** will not be stored in LinkoExchange as those data elements are not currently supported, but when support is added for these columns, the data will import automatically.
-Columns indicated with ** can be excluded from the file completely if desired.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">This is used to identify the differences between the various samples an Industry takes. What is required here is defined by the Authority.  See the </t>
+      <t xml:space="preserve">  Some Required fields can be left blank if the row contains the Flow result that is being used to calculate Mass Loadings.  See Mass Loadings below for more information.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Only concentration results should be imported. Mass loading results will be calculated automatically in LinkoExchange if a mass loading flow is included in the file import or entered into the Draft Sample in LinkoExchange.  See </t>
     </r>
     <r>
       <rPr>
@@ -762,18 +1148,66 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Authority Settings</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> tab for a list of valid Sample Types and consult the Industry or Authority on when to use a particular type.
-Sample Type is a </t>
+      <t xml:space="preserve">Mass Loadings </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>below for more information.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If you are required to report Mass Loadings to your Authority, LinkoExchange can calculate them for you automatically during data import when you include a row for the same unique sample that contains the mass loading flow result.
+To do this, the data in the fields that identify a unique sample (See </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Identifying Unique Samples</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> above) must be identical to those that need to have Mass Loadings calculated.  See the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Data Example with Mass Loadings</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tab for an example of how to include a row with a Mass Loading Flow parameter.
+If any of these fields are identified as Required (MonitoringPoint, CollectionMethod, SampleType, SampleStartDateTime, SampleEndDateTime, LabSampleID, Result, ResultUnit), then the Mass Loading Flow parameter </t>
     </r>
     <r>
       <rPr>
@@ -784,443 +1218,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Recommended</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> field, see </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Recommended Fields</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> above for more details.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>LinkoExchange will accept the following combinations of values for the Result and Result Qualifier fields</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>depending on the Authorities settings:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-     </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Result</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> =  0.098 (any numeric value) and </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Result Qualifier</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is blank
-     </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Result</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> =  0.098 (any numeric value) and </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Result Qualifier</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is &lt; (result is less than 0.098 detection limit)
-     </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Result</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> =  200 (any numeric value) and </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Result Qualifier</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is &gt; (result is greater than 200 detection limit)
-     </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Result</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = blank and </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Result Qualifier</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is ND (for non detect)
-     </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Result</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = blank and </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Result Qualifier</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is NF (for no flow, no sample taken)
-The combinations allowed is determined by the Authority.  See the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Authority Settings </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>tab for a list of valid Result Qualifiers.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Only concentration results should be imported. Mass loading results will be calculated automatically in LinkoExchange if a flow is included in the file import or entered into the Draft Sample in LinkoExchange.  See </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Mass Loadings </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>below for more information.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">&lt;orgname&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>accepts the following values for these fields.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">See the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Data Rules</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> tab for more details.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">If you are required to report Mass Loadings to your Authority, LinkoExchange can calculate them for you automatically during data import when you include a row for the same unique sample that contains the flow result.
-To do this, the data in the fields that identify a unique sample (See </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Identifying Unique Samples</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> above) must be identical to those that need to have Mass Loadings calculated.  See the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Data Example with Mass Loadings</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> tab for an example of how to include a row with a Flow parameter.
-If any of these fields are identified as Required (MonitoringPoint, CollectionMethod, SampleType, SampleStartDateTime, SampleEndDateTime, LabSampleID, Result, ResultUnit), then the Flow parameter </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>must</t>
     </r>
     <r>
@@ -1231,7 +1228,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> have data in that field.  If any other fields are identified as Required, they will be ignored for the Flow parameter.  ResultQualifier is always ignored for the Flow parameter.
+      <t xml:space="preserve"> have data in that field.  If any other fields are identified as Required, they will be ignored for the Mass Loading Flow parameter.  ResultQualifier is always ignored for the Mass Loading Flow parameter.
 </t>
     </r>
     <r>
@@ -1254,6 +1251,9 @@
       </rPr>
       <t xml:space="preserve"> In some rare cases, the Authority may ask you to import Mass Loading Results as Concentration Results by placing the mass result and unit into the Result and ResultUnit fields.  Consult with the Authority to determine if this applies to you.</t>
     </r>
+  </si>
+  <si>
+    <t>MassLoadingFlow</t>
   </si>
 </sst>
 </file>
@@ -1912,25 +1912,25 @@
   <sheetData>
     <row r="1" spans="1:7" s="27" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="C1" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="D1" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="E1" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="F1" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="G1" s="26" t="s">
         <v>79</v>
-      </c>
-      <c r="G1" s="26" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1938,22 +1938,22 @@
         <v>8</v>
       </c>
       <c r="B2" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="30" t="s">
         <v>81</v>
-      </c>
-      <c r="C2" s="30" t="s">
-        <v>82</v>
       </c>
       <c r="D2" s="31">
         <v>25</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F2" s="33" t="s">
         <v>19</v>
       </c>
       <c r="G2" s="34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="51" x14ac:dyDescent="0.2">
@@ -1961,22 +1961,22 @@
         <v>9</v>
       </c>
       <c r="B3" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="30" t="s">
         <v>81</v>
-      </c>
-      <c r="C3" s="30" t="s">
-        <v>82</v>
       </c>
       <c r="D3" s="31">
         <v>25</v>
       </c>
       <c r="E3" s="36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F3" s="37" t="s">
         <v>23</v>
       </c>
       <c r="G3" s="34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
@@ -1984,22 +1984,22 @@
         <v>1</v>
       </c>
       <c r="B4" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="30" t="s">
         <v>81</v>
-      </c>
-      <c r="C4" s="30" t="s">
-        <v>82</v>
       </c>
       <c r="D4" s="31">
         <v>25</v>
       </c>
       <c r="E4" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="F4" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="F4" s="38" t="s">
+      <c r="G4" s="34" t="s">
         <v>87</v>
-      </c>
-      <c r="G4" s="34" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
@@ -2007,20 +2007,20 @@
         <v>10</v>
       </c>
       <c r="B5" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="30" t="s">
         <v>89</v>
-      </c>
-      <c r="C5" s="30" t="s">
-        <v>90</v>
       </c>
       <c r="D5" s="31"/>
       <c r="E5" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="F5" s="39" t="s">
-        <v>92</v>
-      </c>
       <c r="G5" s="40" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
@@ -2028,20 +2028,20 @@
         <v>11</v>
       </c>
       <c r="B6" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="30" t="s">
         <v>89</v>
-      </c>
-      <c r="C6" s="30" t="s">
-        <v>90</v>
       </c>
       <c r="D6" s="31"/>
       <c r="E6" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="F6" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="F6" s="39" t="s">
-        <v>94</v>
-      </c>
       <c r="G6" s="40" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -2049,16 +2049,16 @@
         <v>16</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D7" s="31">
         <v>60</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F7" s="41" t="s">
         <v>6</v>
@@ -2069,22 +2069,22 @@
         <v>17</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D8" s="31">
         <v>2</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F8" s="43" t="s">
         <v>18</v>
       </c>
       <c r="G8" s="32" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -2092,40 +2092,40 @@
         <v>14</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D9" s="31"/>
       <c r="E9" s="32" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F9" s="41">
         <v>0.1</v>
       </c>
       <c r="G9" s="32" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D10" s="31">
         <v>10</v>
       </c>
       <c r="E10" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="F10" s="41" t="s">
         <v>101</v>
-      </c>
-      <c r="F10" s="41" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
@@ -2133,62 +2133,62 @@
         <v>3</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D11" s="31">
         <v>25</v>
       </c>
       <c r="E11" s="36" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F11" s="41" t="s">
         <v>2</v>
       </c>
       <c r="G11" s="40" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D12" s="31">
         <v>100</v>
       </c>
       <c r="E12" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="F12" s="44" t="s">
         <v>106</v>
-      </c>
-      <c r="F12" s="44" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D13" s="31">
         <v>15</v>
       </c>
       <c r="E13" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="F13" s="41" t="s">
         <v>109</v>
-      </c>
-      <c r="F13" s="41" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -2196,16 +2196,16 @@
         <v>15</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D14" s="31">
         <v>10</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F14" s="41">
         <v>5.0000000000000001E-4</v>
@@ -2213,19 +2213,19 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B15" s="30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D15" s="31">
         <v>10</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F15" s="41">
         <v>1E-3</v>
@@ -2236,17 +2236,17 @@
         <v>12</v>
       </c>
       <c r="B16" s="30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D16" s="45"/>
       <c r="E16" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="F16" s="39" t="s">
         <v>114</v>
-      </c>
-      <c r="F16" s="39" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -2254,16 +2254,16 @@
         <v>13</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D17" s="31">
         <v>15</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F17" s="41" t="s">
         <v>5</v>
@@ -2271,38 +2271,38 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B18" s="30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D18" s="31">
         <v>25</v>
       </c>
       <c r="E18" s="34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F18" s="46" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G18" s="47"/>
     </row>
     <row r="19" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="B19" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19" s="30" t="s">
         <v>119</v>
-      </c>
-      <c r="B19" s="30" t="s">
-        <v>103</v>
-      </c>
-      <c r="C19" s="30" t="s">
-        <v>120</v>
       </c>
       <c r="D19" s="31"/>
       <c r="E19" s="32" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F19" s="41">
         <v>1</v>
@@ -2310,121 +2310,121 @@
     </row>
     <row r="20" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B20" s="30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C20" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D20" s="31">
         <v>25</v>
       </c>
       <c r="E20" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="F20" s="41" t="s">
         <v>123</v>
-      </c>
-      <c r="F20" s="41" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B21" s="30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C21" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D21" s="31">
         <v>500</v>
       </c>
       <c r="E21" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="F21" s="41" t="s">
         <v>126</v>
-      </c>
-      <c r="F21" s="41" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C22" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D22" s="31">
         <v>500</v>
       </c>
       <c r="E22" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="F22" s="41" t="s">
         <v>129</v>
-      </c>
-      <c r="F22" s="41" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D23" s="31">
         <v>15</v>
       </c>
       <c r="E23" s="32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F23" s="44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B24" s="30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C24" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D24" s="48">
         <v>25</v>
       </c>
       <c r="E24" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F24" s="46" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G24" s="47"/>
     </row>
     <row r="25" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B25" s="30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C25" s="30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D25" s="31"/>
       <c r="E25" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="F25" s="49" t="s">
         <v>136</v>
-      </c>
-      <c r="F25" s="49" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -2436,19 +2436,19 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="51" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G27" s="47"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G28" s="47"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G29" s="47"/>
     </row>
@@ -2471,12 +2471,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -2485,496 +2485,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:X25"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="14" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.85546875" style="11" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14" style="13" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="21.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16" style="13" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="17.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="9.140625" style="13"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="52" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="53" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="53" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="54" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="55" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="53" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="53" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="53" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="53" t="s">
-        <v>100</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="L1" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="M1" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="N1" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="R1" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="S1" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="T1" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="U1" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="V1" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="X1" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="12">
-        <v>43084.375</v>
-      </c>
-      <c r="E2" s="12">
-        <v>43085.375</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="N2" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="O2" s="12">
-        <v>43090.604166666664</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q2" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="R2" s="13">
-        <v>0</v>
-      </c>
-      <c r="S2" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="T2" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="U2" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="V2" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="W2" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="X2" s="12">
-        <v>43090.708333333336</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="12">
-        <v>43084.375</v>
-      </c>
-      <c r="E3" s="12">
-        <v>43085.375</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="L3" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="M3" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="N3" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="O3" s="12">
-        <v>43090.604166666664</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q3" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="R3" s="13">
-        <v>0</v>
-      </c>
-      <c r="S3" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="T3" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="U3" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="V3" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="W3" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="X3" s="12">
-        <v>43090.708333333336</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="12">
-        <v>43074.625</v>
-      </c>
-      <c r="E4" s="12">
-        <v>43075.625</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="L4" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="M4" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="N4" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="O4" s="12">
-        <v>43080.625</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q4" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="R4" s="13">
-        <v>0</v>
-      </c>
-      <c r="S4" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="T4" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="U4" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="V4" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="W4" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="X4" s="12">
-        <v>43081.708333333336</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="12">
-        <v>43074.625</v>
-      </c>
-      <c r="E5" s="12">
-        <v>43075.625</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="L5" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="M5" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="N5" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="O5" s="12">
-        <v>43080.625</v>
-      </c>
-      <c r="P5" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q5" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="R5" s="13">
-        <v>0</v>
-      </c>
-      <c r="S5" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="T5" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="U5" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="V5" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="W5" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="X5" s="12">
-        <v>43081.708333333336</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="12">
-        <v>43074.625</v>
-      </c>
-      <c r="E6" s="12">
-        <v>43075.625</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="K6" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="L6" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="M6" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="N6" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="O6" s="12">
-        <v>43080.625</v>
-      </c>
-      <c r="P6" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q6" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="R6" s="13">
-        <v>0</v>
-      </c>
-      <c r="S6" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="T6" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="U6" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="V6" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="W6" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="X6" s="12">
-        <v>43081.708333333336</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A25" s="15"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -2990,12 +2500,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:1" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -3003,12 +2513,12 @@
     </row>
     <row r="4" spans="1:1" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:1" s="21" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -3034,7 +2544,7 @@
     </row>
     <row r="11" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
@@ -3057,7 +2567,7 @@
     </row>
     <row r="17" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
@@ -3070,7 +2580,7 @@
     </row>
     <row r="20" spans="1:1" ht="135" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
@@ -3080,7 +2590,7 @@
     </row>
     <row r="23" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
@@ -3090,7 +2600,7 @@
     </row>
     <row r="26" spans="1:1" ht="180" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -3099,56 +2609,30 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="180.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" style="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.5703125" style="13" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.140625" style="11" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9.85546875" style="13" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9.5703125" style="13" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="14" style="13" bestFit="1" customWidth="1"/>
@@ -3186,22 +2670,22 @@
         <v>14</v>
       </c>
       <c r="I1" s="53" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J1" s="6" t="s">
         <v>3</v>
       </c>
       <c r="K1" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="16" t="s">
         <v>50</v>
-      </c>
-      <c r="L1" s="16" t="s">
-        <v>51</v>
       </c>
       <c r="M1" s="15" t="s">
         <v>15</v>
       </c>
       <c r="N1" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O1" s="5" t="s">
         <v>12</v>
@@ -3210,28 +2694,28 @@
         <v>13</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="R1" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="R1" s="15" t="s">
+      <c r="S1" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="S1" s="15" t="s">
+      <c r="T1" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="U1" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="V1" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="W1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="15" t="s">
         <v>59</v>
-      </c>
-      <c r="X1" s="15" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.2">
@@ -3266,16 +2750,16 @@
         <v>33</v>
       </c>
       <c r="K2" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="L2" s="13" t="s">
         <v>61</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>62</v>
       </c>
       <c r="M2" s="11" t="s">
         <v>43</v>
       </c>
       <c r="N2" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O2" s="12">
         <v>43090.604166666664</v>
@@ -3284,25 +2768,25 @@
         <v>39</v>
       </c>
       <c r="Q2" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="R2" s="13">
         <v>0</v>
       </c>
       <c r="S2" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="T2" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="T2" s="13" t="s">
+      <c r="U2" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="U2" s="13" t="s">
+      <c r="V2" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="V2" s="13" t="s">
+      <c r="W2" s="13" t="s">
         <v>68</v>
-      </c>
-      <c r="W2" s="13" t="s">
-        <v>69</v>
       </c>
       <c r="X2" s="12">
         <v>43090.708333333336</v>
@@ -3337,16 +2821,16 @@
         <v>33</v>
       </c>
       <c r="K3" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="L3" s="13" t="s">
         <v>61</v>
-      </c>
-      <c r="L3" s="13" t="s">
-        <v>62</v>
       </c>
       <c r="M3" s="11" t="s">
         <v>43</v>
       </c>
       <c r="N3" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O3" s="12">
         <v>43090.604166666664</v>
@@ -3355,25 +2839,25 @@
         <v>39</v>
       </c>
       <c r="Q3" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="R3" s="13">
         <v>0</v>
       </c>
       <c r="S3" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="T3" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="T3" s="13" t="s">
+      <c r="U3" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="U3" s="13" t="s">
+      <c r="V3" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="V3" s="13" t="s">
+      <c r="W3" s="13" t="s">
         <v>68</v>
-      </c>
-      <c r="W3" s="13" t="s">
-        <v>69</v>
       </c>
       <c r="X3" s="12">
         <v>43090.708333333336</v>
@@ -3411,16 +2895,16 @@
         <v>2</v>
       </c>
       <c r="K4" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="L4" s="13" t="s">
         <v>70</v>
-      </c>
-      <c r="L4" s="13" t="s">
-        <v>71</v>
       </c>
       <c r="M4" s="11" t="s">
         <v>29</v>
       </c>
       <c r="N4" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O4" s="12">
         <v>43080.625</v>
@@ -3429,25 +2913,25 @@
         <v>5</v>
       </c>
       <c r="Q4" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="R4" s="13">
         <v>0</v>
       </c>
       <c r="S4" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="T4" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="U4" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="U4" s="13" t="s">
+      <c r="V4" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="V4" s="13" t="s">
+      <c r="W4" s="13" t="s">
         <v>68</v>
-      </c>
-      <c r="W4" s="13" t="s">
-        <v>69</v>
       </c>
       <c r="X4" s="12">
         <v>43081.708333333336</v>
@@ -3482,16 +2966,16 @@
         <v>2</v>
       </c>
       <c r="K5" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="L5" s="13" t="s">
         <v>70</v>
-      </c>
-      <c r="L5" s="13" t="s">
-        <v>71</v>
       </c>
       <c r="M5" s="11" t="s">
         <v>29</v>
       </c>
       <c r="N5" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O5" s="12">
         <v>43080.625</v>
@@ -3500,25 +2984,25 @@
         <v>5</v>
       </c>
       <c r="Q5" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="R5" s="13">
         <v>0</v>
       </c>
       <c r="S5" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="T5" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="U5" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="U5" s="13" t="s">
+      <c r="V5" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="V5" s="13" t="s">
+      <c r="W5" s="13" t="s">
         <v>68</v>
-      </c>
-      <c r="W5" s="13" t="s">
-        <v>69</v>
       </c>
       <c r="X5" s="12">
         <v>43081.708333333336</v>
@@ -3553,16 +3037,16 @@
         <v>2</v>
       </c>
       <c r="K6" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="L6" s="13" t="s">
         <v>70</v>
-      </c>
-      <c r="L6" s="13" t="s">
-        <v>71</v>
       </c>
       <c r="M6" s="11" t="s">
         <v>29</v>
       </c>
       <c r="N6" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O6" s="12">
         <v>43080.625</v>
@@ -3571,87 +3055,31 @@
         <v>5</v>
       </c>
       <c r="Q6" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="R6" s="13">
         <v>0</v>
       </c>
       <c r="S6" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="T6" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="U6" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="U6" s="13" t="s">
+      <c r="V6" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="V6" s="13" t="s">
+      <c r="W6" s="13" t="s">
         <v>68</v>
-      </c>
-      <c r="W6" s="13" t="s">
-        <v>69</v>
       </c>
       <c r="X6" s="12">
         <v>43081.708333333336</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A7" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="19">
-        <v>43074.625</v>
-      </c>
-      <c r="E7" s="19">
-        <v>43075.625</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="I7" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="J7" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="K7" s="18"/>
-      <c r="L7" s="25"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="19"/>
-      <c r="P7" s="20"/>
-      <c r="Q7" s="25"/>
-      <c r="R7" s="25">
-        <v>0</v>
-      </c>
-      <c r="S7" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="T7" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="U7" s="25"/>
-      <c r="V7" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="W7" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="X7" s="19">
-        <v>43081.708333333336</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="15"/>
       <c r="B25" s="16"/>
       <c r="C25" s="15"/>
@@ -3662,11 +3090,587 @@
       <c r="H25" s="15"/>
       <c r="I25" s="15"/>
       <c r="J25" s="15"/>
+      <c r="K25" s="1"/>
       <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
+      <c r="O25" s="15"/>
+      <c r="P25" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:X25"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16" style="13" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="17.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="9.140625" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="54" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="55" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="53" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="53" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="53" t="s">
+        <v>99</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="R1" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="S1" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="T1" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="U1" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="V1" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="X1" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="12">
+        <v>43084.375</v>
+      </c>
+      <c r="E2" s="12">
+        <v>43085.375</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="O2" s="12">
+        <v>43090.604166666664</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q2" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="R2" s="13">
+        <v>0</v>
+      </c>
+      <c r="S2" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="T2" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="U2" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="V2" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="W2" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="X2" s="12">
+        <v>43090.708333333336</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="12">
+        <v>43084.375</v>
+      </c>
+      <c r="E3" s="12">
+        <v>43085.375</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="M3" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="O3" s="12">
+        <v>43090.604166666664</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q3" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="R3" s="13">
+        <v>0</v>
+      </c>
+      <c r="S3" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="T3" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="U3" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="V3" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="W3" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="X3" s="12">
+        <v>43090.708333333336</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="12">
+        <v>43074.625</v>
+      </c>
+      <c r="E4" s="12">
+        <v>43075.625</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="L4" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="O4" s="12">
+        <v>43080.625</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q4" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="R4" s="13">
+        <v>0</v>
+      </c>
+      <c r="S4" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="T4" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="U4" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="V4" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="W4" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="X4" s="12">
+        <v>43081.708333333336</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="12">
+        <v>43074.625</v>
+      </c>
+      <c r="E5" s="12">
+        <v>43075.625</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="O5" s="12">
+        <v>43080.625</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q5" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="R5" s="13">
+        <v>0</v>
+      </c>
+      <c r="S5" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="T5" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="U5" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="V5" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="W5" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="X5" s="12">
+        <v>43081.708333333336</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="12">
+        <v>43074.625</v>
+      </c>
+      <c r="E6" s="12">
+        <v>43075.625</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="L6" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="N6" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="O6" s="12">
+        <v>43080.625</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q6" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="R6" s="13">
+        <v>0</v>
+      </c>
+      <c r="S6" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="T6" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="U6" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="V6" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="W6" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="X6" s="12">
+        <v>43081.708333333336</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A7" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="19">
+        <v>43074.625</v>
+      </c>
+      <c r="E7" s="19">
+        <v>43075.625</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="18"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="25"/>
+      <c r="R7" s="25">
+        <v>0</v>
+      </c>
+      <c r="S7" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="T7" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="U7" s="25"/>
+      <c r="V7" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="W7" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="X7" s="19">
+        <v>43081.708333333336</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A25" s="15"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="15"/>
+      <c r="O25" s="15"/>
+      <c r="P25" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="180.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the instruction template.
TFS Changeset 2418: http://wtrxtfs2013.watertrax.local:8080/tfs/Linko/LinkoApplications/_versionControl/changeset/2418 

Workitems:
[8480] Coding - User Story 8185:Both Portals - Create dynamic template instruction xlsx file
TFS: http://wtrxtfs2013.watertrax.local:8080/tfs/Linko/WorkItemTracking/WorkItem.aspx?artifactMoniker=8480 
Jira: https://aquaticinformatics.atlassian.net/issues/?jql=project%20%3D%20LINKO%20and%20tfsissueid~8480
</commit_message>
<xml_diff>
--- a/Linko.LinkoExchange.Web/Resources/SampleImportInstruction.xlsx
+++ b/Linko.LinkoExchange.Web/Resources/SampleImportInstruction.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\LinkoApplications\Development\LinkoExchange\Linko.LinkoExchange.Web\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{17F2FD19-6F23-4EE6-9708-CEFBBE6F1C61}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{04567AD4-B16B-4099-BF38-DE59A5F64B7F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9135" tabRatio="764" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -173,76 +173,6 @@
     <t>10</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">These fields are not required but are strongly recommended to simplify data import.  Sample results cannot be imported into LinkoExchange without this data.  If it is not included in the file, the LinkoExchange user will be prompted to choose this data during the import process.  
-If the data </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>can</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> be included in the file, then the file can contain sample results for multiple Monitoring Points, Collection Methods and Sample Types.  
-If the data </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>cannot</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> be included in the file, then the file </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>must</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> only contain data for a single Monitoring Point, Collection Method and Sample Type.</t>
-    </r>
-  </si>
-  <si>
     <t>LinkoExchange identifies unique samples using the following 6 fields:  MonitoringPoint, CollectionMethod, SampleType, SampleStartDateTime, SampleEndDateTime, LabSampleID
 A file can contain results for multiple samples and LinkoExchange will automatically group those results into Samples using these fields.</t>
   </si>
@@ -1254,6 +1184,11 @@
   </si>
   <si>
     <t>MassLoadingFlow</t>
+  </si>
+  <si>
+    <t>These fields are not required but are strongly recommended to simplify data import.  If these fields are not included in the file, the LinkoExchange user will be prompted to choose this data during the import process.  
+If data is included for these fields in the file, then the file can contain sample results for multiple Monitoring Points, Collection Methods and Sample Types.
+If data is not included for any of these fields in the file, then the file must only contain data for a single Monitoring Point, Collection Method and Sample Type.</t>
   </si>
 </sst>
 </file>
@@ -1263,7 +1198,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy\ h:mm\ AM/PM"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1308,14 +1243,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1506,109 +1433,109 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="22" fontId="15" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="22" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1912,25 +1839,25 @@
   <sheetData>
     <row r="1" spans="1:7" s="27" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="C1" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="D1" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="E1" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="F1" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="G1" s="26" t="s">
         <v>78</v>
-      </c>
-      <c r="G1" s="26" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1938,22 +1865,22 @@
         <v>8</v>
       </c>
       <c r="B2" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="30" t="s">
         <v>80</v>
-      </c>
-      <c r="C2" s="30" t="s">
-        <v>81</v>
       </c>
       <c r="D2" s="31">
         <v>25</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F2" s="33" t="s">
         <v>19</v>
       </c>
       <c r="G2" s="34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="51" x14ac:dyDescent="0.2">
@@ -1961,22 +1888,22 @@
         <v>9</v>
       </c>
       <c r="B3" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="30" t="s">
         <v>80</v>
-      </c>
-      <c r="C3" s="30" t="s">
-        <v>81</v>
       </c>
       <c r="D3" s="31">
         <v>25</v>
       </c>
       <c r="E3" s="36" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F3" s="37" t="s">
         <v>23</v>
       </c>
       <c r="G3" s="34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
@@ -1984,22 +1911,22 @@
         <v>1</v>
       </c>
       <c r="B4" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="30" t="s">
         <v>80</v>
-      </c>
-      <c r="C4" s="30" t="s">
-        <v>81</v>
       </c>
       <c r="D4" s="31">
         <v>25</v>
       </c>
       <c r="E4" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="F4" s="38" t="s">
+      <c r="G4" s="34" t="s">
         <v>86</v>
-      </c>
-      <c r="G4" s="34" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
@@ -2007,20 +1934,20 @@
         <v>10</v>
       </c>
       <c r="B5" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="30" t="s">
         <v>88</v>
-      </c>
-      <c r="C5" s="30" t="s">
-        <v>89</v>
       </c>
       <c r="D5" s="31"/>
       <c r="E5" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="F5" s="39" t="s">
-        <v>91</v>
-      </c>
       <c r="G5" s="40" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
@@ -2028,20 +1955,20 @@
         <v>11</v>
       </c>
       <c r="B6" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="30" t="s">
         <v>88</v>
-      </c>
-      <c r="C6" s="30" t="s">
-        <v>89</v>
       </c>
       <c r="D6" s="31"/>
       <c r="E6" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="F6" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="F6" s="39" t="s">
-        <v>93</v>
-      </c>
       <c r="G6" s="40" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -2049,16 +1976,16 @@
         <v>16</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D7" s="31">
         <v>60</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F7" s="41" t="s">
         <v>6</v>
@@ -2069,22 +1996,22 @@
         <v>17</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D8" s="31">
         <v>2</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F8" s="43" t="s">
         <v>18</v>
       </c>
       <c r="G8" s="32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -2092,40 +2019,40 @@
         <v>14</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D9" s="31"/>
       <c r="E9" s="32" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F9" s="41">
         <v>0.1</v>
       </c>
       <c r="G9" s="32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10" s="35" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D10" s="31">
         <v>10</v>
       </c>
       <c r="E10" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="F10" s="41" t="s">
         <v>100</v>
-      </c>
-      <c r="F10" s="41" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
@@ -2133,62 +2060,62 @@
         <v>3</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D11" s="31">
         <v>25</v>
       </c>
       <c r="E11" s="36" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F11" s="41" t="s">
         <v>2</v>
       </c>
       <c r="G11" s="40" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D12" s="31">
         <v>100</v>
       </c>
       <c r="E12" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="F12" s="44" t="s">
         <v>105</v>
-      </c>
-      <c r="F12" s="44" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D13" s="31">
         <v>15</v>
       </c>
       <c r="E13" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="F13" s="41" t="s">
         <v>108</v>
-      </c>
-      <c r="F13" s="41" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -2196,16 +2123,16 @@
         <v>15</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D14" s="31">
         <v>10</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F14" s="41">
         <v>5.0000000000000001E-4</v>
@@ -2213,19 +2140,19 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B15" s="30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D15" s="31">
         <v>10</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F15" s="41">
         <v>1E-3</v>
@@ -2236,17 +2163,17 @@
         <v>12</v>
       </c>
       <c r="B16" s="30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D16" s="45"/>
       <c r="E16" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="F16" s="39" t="s">
         <v>113</v>
-      </c>
-      <c r="F16" s="39" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -2254,16 +2181,16 @@
         <v>13</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D17" s="31">
         <v>15</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F17" s="41" t="s">
         <v>5</v>
@@ -2271,38 +2198,38 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B18" s="30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D18" s="31">
         <v>25</v>
       </c>
       <c r="E18" s="34" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F18" s="46" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G18" s="47"/>
     </row>
     <row r="19" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="B19" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="C19" s="30" t="s">
         <v>118</v>
-      </c>
-      <c r="B19" s="30" t="s">
-        <v>102</v>
-      </c>
-      <c r="C19" s="30" t="s">
-        <v>119</v>
       </c>
       <c r="D19" s="31"/>
       <c r="E19" s="32" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F19" s="41">
         <v>1</v>
@@ -2310,121 +2237,121 @@
     </row>
     <row r="20" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B20" s="30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C20" s="30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D20" s="31">
         <v>25</v>
       </c>
       <c r="E20" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="F20" s="41" t="s">
         <v>122</v>
-      </c>
-      <c r="F20" s="41" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B21" s="30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C21" s="30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D21" s="31">
         <v>500</v>
       </c>
       <c r="E21" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="F21" s="41" t="s">
         <v>125</v>
-      </c>
-      <c r="F21" s="41" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C22" s="30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D22" s="31">
         <v>500</v>
       </c>
       <c r="E22" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="F22" s="41" t="s">
         <v>128</v>
-      </c>
-      <c r="F22" s="41" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D23" s="31">
         <v>15</v>
       </c>
       <c r="E23" s="32" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F23" s="44" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B24" s="30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C24" s="30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D24" s="48">
         <v>25</v>
       </c>
       <c r="E24" s="34" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F24" s="46" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G24" s="47"/>
     </row>
     <row r="25" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B25" s="30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C25" s="30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D25" s="31"/>
       <c r="E25" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="F25" s="49" t="s">
         <v>135</v>
-      </c>
-      <c r="F25" s="49" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -2436,19 +2363,19 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="51" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G27" s="47"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G28" s="47"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G29" s="47"/>
     </row>
@@ -2471,12 +2398,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -2500,12 +2427,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:1" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -2513,12 +2440,12 @@
     </row>
     <row r="4" spans="1:1" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:1" s="21" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -2531,7 +2458,7 @@
     </row>
     <row r="8" spans="1:1" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>44</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
@@ -2544,7 +2471,7 @@
     </row>
     <row r="11" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
@@ -2557,7 +2484,7 @@
     </row>
     <row r="14" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
@@ -2567,7 +2494,7 @@
     </row>
     <row r="17" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
@@ -2580,7 +2507,7 @@
     </row>
     <row r="20" spans="1:1" ht="135" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
@@ -2590,7 +2517,7 @@
     </row>
     <row r="23" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
@@ -2600,7 +2527,7 @@
     </row>
     <row r="26" spans="1:1" ht="180" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -2670,22 +2597,22 @@
         <v>14</v>
       </c>
       <c r="I1" s="53" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J1" s="6" t="s">
         <v>3</v>
       </c>
       <c r="K1" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="L1" s="16" t="s">
         <v>49</v>
-      </c>
-      <c r="L1" s="16" t="s">
-        <v>50</v>
       </c>
       <c r="M1" s="15" t="s">
         <v>15</v>
       </c>
       <c r="N1" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O1" s="5" t="s">
         <v>12</v>
@@ -2694,28 +2621,28 @@
         <v>13</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R1" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="R1" s="15" t="s">
+      <c r="S1" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="S1" s="15" t="s">
+      <c r="T1" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="U1" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="V1" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="W1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="15" t="s">
         <v>58</v>
-      </c>
-      <c r="X1" s="15" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.2">
@@ -2750,16 +2677,16 @@
         <v>33</v>
       </c>
       <c r="K2" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="L2" s="13" t="s">
         <v>60</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>61</v>
       </c>
       <c r="M2" s="11" t="s">
         <v>43</v>
       </c>
       <c r="N2" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O2" s="12">
         <v>43090.604166666664</v>
@@ -2768,25 +2695,25 @@
         <v>39</v>
       </c>
       <c r="Q2" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R2" s="13">
         <v>0</v>
       </c>
       <c r="S2" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="T2" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="T2" s="13" t="s">
+      <c r="U2" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="U2" s="13" t="s">
+      <c r="V2" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="V2" s="13" t="s">
+      <c r="W2" s="13" t="s">
         <v>67</v>
-      </c>
-      <c r="W2" s="13" t="s">
-        <v>68</v>
       </c>
       <c r="X2" s="12">
         <v>43090.708333333336</v>
@@ -2821,16 +2748,16 @@
         <v>33</v>
       </c>
       <c r="K3" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="L3" s="13" t="s">
         <v>60</v>
-      </c>
-      <c r="L3" s="13" t="s">
-        <v>61</v>
       </c>
       <c r="M3" s="11" t="s">
         <v>43</v>
       </c>
       <c r="N3" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O3" s="12">
         <v>43090.604166666664</v>
@@ -2839,25 +2766,25 @@
         <v>39</v>
       </c>
       <c r="Q3" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R3" s="13">
         <v>0</v>
       </c>
       <c r="S3" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="T3" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="T3" s="13" t="s">
+      <c r="U3" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="U3" s="13" t="s">
+      <c r="V3" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="V3" s="13" t="s">
+      <c r="W3" s="13" t="s">
         <v>67</v>
-      </c>
-      <c r="W3" s="13" t="s">
-        <v>68</v>
       </c>
       <c r="X3" s="12">
         <v>43090.708333333336</v>
@@ -2895,16 +2822,16 @@
         <v>2</v>
       </c>
       <c r="K4" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="L4" s="13" t="s">
         <v>69</v>
-      </c>
-      <c r="L4" s="13" t="s">
-        <v>70</v>
       </c>
       <c r="M4" s="11" t="s">
         <v>29</v>
       </c>
       <c r="N4" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O4" s="12">
         <v>43080.625</v>
@@ -2913,25 +2840,25 @@
         <v>5</v>
       </c>
       <c r="Q4" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R4" s="13">
         <v>0</v>
       </c>
       <c r="S4" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="T4" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="U4" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="U4" s="13" t="s">
+      <c r="V4" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="V4" s="13" t="s">
+      <c r="W4" s="13" t="s">
         <v>67</v>
-      </c>
-      <c r="W4" s="13" t="s">
-        <v>68</v>
       </c>
       <c r="X4" s="12">
         <v>43081.708333333336</v>
@@ -2966,16 +2893,16 @@
         <v>2</v>
       </c>
       <c r="K5" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="L5" s="13" t="s">
         <v>69</v>
-      </c>
-      <c r="L5" s="13" t="s">
-        <v>70</v>
       </c>
       <c r="M5" s="11" t="s">
         <v>29</v>
       </c>
       <c r="N5" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O5" s="12">
         <v>43080.625</v>
@@ -2984,25 +2911,25 @@
         <v>5</v>
       </c>
       <c r="Q5" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R5" s="13">
         <v>0</v>
       </c>
       <c r="S5" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="T5" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="U5" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="U5" s="13" t="s">
+      <c r="V5" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="V5" s="13" t="s">
+      <c r="W5" s="13" t="s">
         <v>67</v>
-      </c>
-      <c r="W5" s="13" t="s">
-        <v>68</v>
       </c>
       <c r="X5" s="12">
         <v>43081.708333333336</v>
@@ -3037,16 +2964,16 @@
         <v>2</v>
       </c>
       <c r="K6" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="L6" s="13" t="s">
         <v>69</v>
-      </c>
-      <c r="L6" s="13" t="s">
-        <v>70</v>
       </c>
       <c r="M6" s="11" t="s">
         <v>29</v>
       </c>
       <c r="N6" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O6" s="12">
         <v>43080.625</v>
@@ -3055,25 +2982,25 @@
         <v>5</v>
       </c>
       <c r="Q6" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R6" s="13">
         <v>0</v>
       </c>
       <c r="S6" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="T6" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="U6" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="U6" s="13" t="s">
+      <c r="V6" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="V6" s="13" t="s">
+      <c r="W6" s="13" t="s">
         <v>67</v>
-      </c>
-      <c r="W6" s="13" t="s">
-        <v>68</v>
       </c>
       <c r="X6" s="12">
         <v>43081.708333333336</v>
@@ -3162,22 +3089,22 @@
         <v>14</v>
       </c>
       <c r="I1" s="53" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J1" s="6" t="s">
         <v>3</v>
       </c>
       <c r="K1" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="L1" s="16" t="s">
         <v>49</v>
-      </c>
-      <c r="L1" s="16" t="s">
-        <v>50</v>
       </c>
       <c r="M1" s="15" t="s">
         <v>15</v>
       </c>
       <c r="N1" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O1" s="5" t="s">
         <v>12</v>
@@ -3186,28 +3113,28 @@
         <v>13</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R1" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="R1" s="15" t="s">
+      <c r="S1" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="S1" s="15" t="s">
+      <c r="T1" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="U1" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="V1" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="W1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="15" t="s">
         <v>58</v>
-      </c>
-      <c r="X1" s="15" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.2">
@@ -3242,16 +3169,16 @@
         <v>33</v>
       </c>
       <c r="K2" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="L2" s="13" t="s">
         <v>60</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>61</v>
       </c>
       <c r="M2" s="11" t="s">
         <v>43</v>
       </c>
       <c r="N2" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O2" s="12">
         <v>43090.604166666664</v>
@@ -3260,25 +3187,25 @@
         <v>39</v>
       </c>
       <c r="Q2" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R2" s="13">
         <v>0</v>
       </c>
       <c r="S2" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="T2" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="T2" s="13" t="s">
+      <c r="U2" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="U2" s="13" t="s">
+      <c r="V2" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="V2" s="13" t="s">
+      <c r="W2" s="13" t="s">
         <v>67</v>
-      </c>
-      <c r="W2" s="13" t="s">
-        <v>68</v>
       </c>
       <c r="X2" s="12">
         <v>43090.708333333336</v>
@@ -3313,16 +3240,16 @@
         <v>33</v>
       </c>
       <c r="K3" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="L3" s="13" t="s">
         <v>60</v>
-      </c>
-      <c r="L3" s="13" t="s">
-        <v>61</v>
       </c>
       <c r="M3" s="11" t="s">
         <v>43</v>
       </c>
       <c r="N3" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O3" s="12">
         <v>43090.604166666664</v>
@@ -3331,25 +3258,25 @@
         <v>39</v>
       </c>
       <c r="Q3" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R3" s="13">
         <v>0</v>
       </c>
       <c r="S3" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="T3" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="T3" s="13" t="s">
+      <c r="U3" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="U3" s="13" t="s">
+      <c r="V3" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="V3" s="13" t="s">
+      <c r="W3" s="13" t="s">
         <v>67</v>
-      </c>
-      <c r="W3" s="13" t="s">
-        <v>68</v>
       </c>
       <c r="X3" s="12">
         <v>43090.708333333336</v>
@@ -3387,16 +3314,16 @@
         <v>2</v>
       </c>
       <c r="K4" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="L4" s="13" t="s">
         <v>69</v>
-      </c>
-      <c r="L4" s="13" t="s">
-        <v>70</v>
       </c>
       <c r="M4" s="11" t="s">
         <v>29</v>
       </c>
       <c r="N4" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O4" s="12">
         <v>43080.625</v>
@@ -3405,25 +3332,25 @@
         <v>5</v>
       </c>
       <c r="Q4" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R4" s="13">
         <v>0</v>
       </c>
       <c r="S4" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="T4" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="U4" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="U4" s="13" t="s">
+      <c r="V4" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="V4" s="13" t="s">
+      <c r="W4" s="13" t="s">
         <v>67</v>
-      </c>
-      <c r="W4" s="13" t="s">
-        <v>68</v>
       </c>
       <c r="X4" s="12">
         <v>43081.708333333336</v>
@@ -3458,16 +3385,16 @@
         <v>2</v>
       </c>
       <c r="K5" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="L5" s="13" t="s">
         <v>69</v>
-      </c>
-      <c r="L5" s="13" t="s">
-        <v>70</v>
       </c>
       <c r="M5" s="11" t="s">
         <v>29</v>
       </c>
       <c r="N5" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O5" s="12">
         <v>43080.625</v>
@@ -3476,25 +3403,25 @@
         <v>5</v>
       </c>
       <c r="Q5" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R5" s="13">
         <v>0</v>
       </c>
       <c r="S5" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="T5" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="U5" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="U5" s="13" t="s">
+      <c r="V5" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="V5" s="13" t="s">
+      <c r="W5" s="13" t="s">
         <v>67</v>
-      </c>
-      <c r="W5" s="13" t="s">
-        <v>68</v>
       </c>
       <c r="X5" s="12">
         <v>43081.708333333336</v>
@@ -3529,16 +3456,16 @@
         <v>2</v>
       </c>
       <c r="K6" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="L6" s="13" t="s">
         <v>69</v>
-      </c>
-      <c r="L6" s="13" t="s">
-        <v>70</v>
       </c>
       <c r="M6" s="11" t="s">
         <v>29</v>
       </c>
       <c r="N6" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O6" s="12">
         <v>43080.625</v>
@@ -3547,25 +3474,25 @@
         <v>5</v>
       </c>
       <c r="Q6" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R6" s="13">
         <v>0</v>
       </c>
       <c r="S6" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="T6" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="U6" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="U6" s="13" t="s">
+      <c r="V6" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="V6" s="13" t="s">
+      <c r="W6" s="13" t="s">
         <v>67</v>
-      </c>
-      <c r="W6" s="13" t="s">
-        <v>68</v>
       </c>
       <c r="X6" s="12">
         <v>43081.708333333336</v>
@@ -3588,11 +3515,11 @@
         <v>43075.625</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G7" s="18"/>
       <c r="H7" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I7" s="18" t="s">
         <v>41</v>
@@ -3611,17 +3538,17 @@
         <v>0</v>
       </c>
       <c r="S7" s="25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="T7" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="U7" s="25"/>
       <c r="V7" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="W7" s="25" t="s">
         <v>67</v>
-      </c>
-      <c r="W7" s="25" t="s">
-        <v>68</v>
       </c>
       <c r="X7" s="19">
         <v>43081.708333333336</v>
@@ -3667,7 +3594,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed wording inside the xlsx file. Fixed typo mistakes and updated code format using resharper.
TFS Changeset 2426: http://wtrxtfs2013.watertrax.local:8080/tfs/Linko/LinkoApplications/_versionControl/changeset/2426 

Workitems:
[8756] Coding - Bug 8755:Change wording Optionality to Required in xlsx instructions
TFS: http://wtrxtfs2013.watertrax.local:8080/tfs/Linko/WorkItemTracking/WorkItem.aspx?artifactMoniker=8756 
Jira: https://aquaticinformatics.atlassian.net/issues/?jql=project%20%3D%20LINKO%20and%20tfsissueid~8756
</commit_message>
<xml_diff>
--- a/Linko.LinkoExchange.Web/Resources/SampleImportInstruction.xlsx
+++ b/Linko.LinkoExchange.Web/Resources/SampleImportInstruction.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\LinkoApplications\Development\LinkoExchange\Linko.LinkoExchange.Web\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{04567AD4-B16B-4099-BF38-DE59A5F64B7F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B3116FF3-FE93-4000-8600-53778DDC0BFE}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9135" tabRatio="764" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -261,9 +261,6 @@
     <t>Column Header</t>
   </si>
   <si>
-    <t>Optionality***</t>
-  </si>
-  <si>
     <t>Data Format</t>
   </si>
   <si>
@@ -1189,6 +1186,9 @@
     <t>These fields are not required but are strongly recommended to simplify data import.  If these fields are not included in the file, the LinkoExchange user will be prompted to choose this data during the import process.  
 If data is included for these fields in the file, then the file can contain sample results for multiple Monitoring Points, Collection Methods and Sample Types.
 If data is not included for any of these fields in the file, then the file must only contain data for a single Monitoring Point, Collection Method and Sample Type.</t>
+  </si>
+  <si>
+    <t>Required***</t>
   </si>
 </sst>
 </file>
@@ -1842,22 +1842,22 @@
         <v>72</v>
       </c>
       <c r="B1" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="D1" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="E1" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="F1" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="G1" s="26" t="s">
         <v>77</v>
-      </c>
-      <c r="G1" s="26" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1865,22 +1865,22 @@
         <v>8</v>
       </c>
       <c r="B2" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="30" t="s">
         <v>79</v>
-      </c>
-      <c r="C2" s="30" t="s">
-        <v>80</v>
       </c>
       <c r="D2" s="31">
         <v>25</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F2" s="33" t="s">
         <v>19</v>
       </c>
       <c r="G2" s="34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="51" x14ac:dyDescent="0.2">
@@ -1888,22 +1888,22 @@
         <v>9</v>
       </c>
       <c r="B3" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="30" t="s">
         <v>79</v>
-      </c>
-      <c r="C3" s="30" t="s">
-        <v>80</v>
       </c>
       <c r="D3" s="31">
         <v>25</v>
       </c>
       <c r="E3" s="36" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F3" s="37" t="s">
         <v>23</v>
       </c>
       <c r="G3" s="34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
@@ -1911,22 +1911,22 @@
         <v>1</v>
       </c>
       <c r="B4" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="30" t="s">
         <v>79</v>
-      </c>
-      <c r="C4" s="30" t="s">
-        <v>80</v>
       </c>
       <c r="D4" s="31">
         <v>25</v>
       </c>
       <c r="E4" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="F4" s="38" t="s">
+      <c r="G4" s="34" t="s">
         <v>85</v>
-      </c>
-      <c r="G4" s="34" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
@@ -1934,20 +1934,20 @@
         <v>10</v>
       </c>
       <c r="B5" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="30" t="s">
         <v>87</v>
-      </c>
-      <c r="C5" s="30" t="s">
-        <v>88</v>
       </c>
       <c r="D5" s="31"/>
       <c r="E5" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="F5" s="39" t="s">
         <v>89</v>
       </c>
-      <c r="F5" s="39" t="s">
-        <v>90</v>
-      </c>
       <c r="G5" s="40" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
@@ -1955,20 +1955,20 @@
         <v>11</v>
       </c>
       <c r="B6" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="30" t="s">
         <v>87</v>
-      </c>
-      <c r="C6" s="30" t="s">
-        <v>88</v>
       </c>
       <c r="D6" s="31"/>
       <c r="E6" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="F6" s="39" t="s">
-        <v>92</v>
-      </c>
       <c r="G6" s="40" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1976,16 +1976,16 @@
         <v>16</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D7" s="31">
         <v>60</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F7" s="41" t="s">
         <v>6</v>
@@ -1996,22 +1996,22 @@
         <v>17</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D8" s="31">
         <v>2</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F8" s="43" t="s">
         <v>18</v>
       </c>
       <c r="G8" s="32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -2019,40 +2019,40 @@
         <v>14</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D9" s="31"/>
       <c r="E9" s="32" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F9" s="41">
         <v>0.1</v>
       </c>
       <c r="G9" s="32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10" s="35" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D10" s="31">
         <v>10</v>
       </c>
       <c r="E10" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="F10" s="41" t="s">
         <v>99</v>
-      </c>
-      <c r="F10" s="41" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
@@ -2060,62 +2060,62 @@
         <v>3</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D11" s="31">
         <v>25</v>
       </c>
       <c r="E11" s="36" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F11" s="41" t="s">
         <v>2</v>
       </c>
       <c r="G11" s="40" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D12" s="31">
         <v>100</v>
       </c>
       <c r="E12" s="36" t="s">
+        <v>103</v>
+      </c>
+      <c r="F12" s="44" t="s">
         <v>104</v>
-      </c>
-      <c r="F12" s="44" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D13" s="31">
         <v>15</v>
       </c>
       <c r="E13" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="F13" s="41" t="s">
         <v>107</v>
-      </c>
-      <c r="F13" s="41" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -2123,16 +2123,16 @@
         <v>15</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D14" s="31">
         <v>10</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F14" s="41">
         <v>5.0000000000000001E-4</v>
@@ -2140,19 +2140,19 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B15" s="30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D15" s="31">
         <v>10</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F15" s="41">
         <v>1E-3</v>
@@ -2163,17 +2163,17 @@
         <v>12</v>
       </c>
       <c r="B16" s="30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D16" s="45"/>
       <c r="E16" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="F16" s="39" t="s">
         <v>112</v>
-      </c>
-      <c r="F16" s="39" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -2181,16 +2181,16 @@
         <v>13</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D17" s="31">
         <v>15</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F17" s="41" t="s">
         <v>5</v>
@@ -2198,19 +2198,19 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B18" s="30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D18" s="31">
         <v>25</v>
       </c>
       <c r="E18" s="34" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F18" s="46" t="s">
         <v>62</v>
@@ -2219,17 +2219,17 @@
     </row>
     <row r="19" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="B19" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="C19" s="30" t="s">
         <v>117</v>
-      </c>
-      <c r="B19" s="30" t="s">
-        <v>101</v>
-      </c>
-      <c r="C19" s="30" t="s">
-        <v>118</v>
       </c>
       <c r="D19" s="31"/>
       <c r="E19" s="32" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F19" s="41">
         <v>1</v>
@@ -2237,79 +2237,79 @@
     </row>
     <row r="20" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B20" s="30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C20" s="30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D20" s="31">
         <v>25</v>
       </c>
       <c r="E20" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="F20" s="41" t="s">
         <v>121</v>
-      </c>
-      <c r="F20" s="41" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B21" s="30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C21" s="30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D21" s="31">
         <v>500</v>
       </c>
       <c r="E21" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="F21" s="41" t="s">
         <v>124</v>
-      </c>
-      <c r="F21" s="41" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C22" s="30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D22" s="31">
         <v>500</v>
       </c>
       <c r="E22" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="F22" s="41" t="s">
         <v>127</v>
-      </c>
-      <c r="F22" s="41" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D23" s="31">
         <v>15</v>
       </c>
       <c r="E23" s="32" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F23" s="44" t="s">
         <v>66</v>
@@ -2317,19 +2317,19 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B24" s="30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C24" s="30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D24" s="48">
         <v>25</v>
       </c>
       <c r="E24" s="34" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F24" s="46" t="s">
         <v>67</v>
@@ -2338,20 +2338,20 @@
     </row>
     <row r="25" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B25" s="30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C25" s="30" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D25" s="31"/>
       <c r="E25" s="32" t="s">
+        <v>133</v>
+      </c>
+      <c r="F25" s="49" t="s">
         <v>134</v>
-      </c>
-      <c r="F25" s="49" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -2363,19 +2363,19 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="51" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G27" s="47"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G28" s="47"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G29" s="47"/>
     </row>
@@ -2398,12 +2398,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -2432,7 +2432,7 @@
     </row>
     <row r="2" spans="1:1" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -2440,12 +2440,12 @@
     </row>
     <row r="4" spans="1:1" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:1" s="21" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -2458,7 +2458,7 @@
     </row>
     <row r="8" spans="1:1" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
@@ -2471,7 +2471,7 @@
     </row>
     <row r="11" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
@@ -2494,7 +2494,7 @@
     </row>
     <row r="17" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
@@ -2507,7 +2507,7 @@
     </row>
     <row r="20" spans="1:1" ht="135" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
@@ -2517,7 +2517,7 @@
     </row>
     <row r="23" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
@@ -2527,7 +2527,7 @@
     </row>
     <row r="26" spans="1:1" ht="180" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -2597,7 +2597,7 @@
         <v>14</v>
       </c>
       <c r="I1" s="53" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J1" s="6" t="s">
         <v>3</v>
@@ -3089,7 +3089,7 @@
         <v>14</v>
       </c>
       <c r="I1" s="53" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J1" s="6" t="s">
         <v>3</v>
@@ -3515,7 +3515,7 @@
         <v>43075.625</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G7" s="18"/>
       <c r="H7" s="18" t="s">

</xml_diff>